<commit_message>
Model and market comparison of hedging strategies
</commit_message>
<xml_diff>
--- a/nsde_2021_calibrations/Dynamic_calibration_hedging/Model_market_hedges_comparison.xlsx
+++ b/nsde_2021_calibrations/Dynamic_calibration_hedging/Model_market_hedges_comparison.xlsx
@@ -95,9 +95,6 @@
     <t>Straddle t=0 Price</t>
   </si>
   <si>
-    <t>no options traded</t>
-  </si>
-  <si>
     <t>Hedge Straddle (Model)</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Hedge Straddle Error (market)</t>
+  </si>
+  <si>
+    <t>no vanilla  options traded with required strike (deltas interpolated to -1 at the last re-balancing date)</t>
   </si>
 </sst>
 </file>
@@ -423,16 +423,16 @@
                   <c:v>43.656583278099788</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43.762752716241494</c:v>
+                  <c:v>43.596128420137347</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43.121337078600732</c:v>
+                  <c:v>43.240524423594934</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44.290949408497227</c:v>
+                  <c:v>43.483368443486484</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.406778541215033</c:v>
+                  <c:v>43.484236772437441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -970,16 +970,16 @@
                   <c:v>2.2827789150410168E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5198431263950855E-2</c:v>
+                  <c:v>2.1472742054428385E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.069858009643374E-2</c:v>
+                  <c:v>1.3425471391326538E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.6823536868783514E-2</c:v>
+                  <c:v>1.8935249796863771E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.0737742609895247E-2</c:v>
+                  <c:v>1.8954840503487495E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2603,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,7 +2655,7 @@
         <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M4" t="s">
         <v>19</v>
@@ -3171,7 +3171,8 @@
         <v>-0.90990000000000004</v>
       </c>
       <c r="M12" s="3">
-        <v>-0.86779167973132199</v>
+        <f>-0.9</f>
+        <v>-0.9</v>
       </c>
       <c r="N12">
         <f t="shared" si="9"/>
@@ -3237,7 +3238,7 @@
         <v>-0.97109999999999996</v>
       </c>
       <c r="M13" s="3">
-        <v>-0.86779167973132199</v>
+        <v>-0.93500000000000005</v>
       </c>
       <c r="N13">
         <f t="shared" si="9"/>
@@ -3303,7 +3304,7 @@
         <v>-0.98970000000000002</v>
       </c>
       <c r="M14" s="3">
-        <v>-0.86779167973132199</v>
+        <v>-0.97</v>
       </c>
       <c r="N14">
         <f t="shared" si="9"/>
@@ -3369,7 +3370,7 @@
         <v>-1</v>
       </c>
       <c r="M15" s="3">
-        <v>-0.86779167973132199</v>
+        <v>-1</v>
       </c>
       <c r="N15">
         <f t="shared" si="9"/>
@@ -3479,17 +3480,16 @@
     </row>
     <row r="18" spans="8:19" x14ac:dyDescent="0.25">
       <c r="K18" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
     </row>
     <row r="21" spans="8:19" x14ac:dyDescent="0.25">
       <c r="S21" s="2"/>
     </row>
     <row r="22" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H22" s="1"/>
-      <c r="O22">
-        <v>-6.4100000000000004E-2</v>
-      </c>
     </row>
     <row r="23" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H23" s="1"/>
@@ -3502,9 +3502,6 @@
       <c r="K23" t="s">
         <v>22</v>
       </c>
-      <c r="O23">
-        <v>-0.52849999999999997</v>
-      </c>
     </row>
     <row r="24" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H24" s="1"/>
@@ -3517,9 +3514,6 @@
       <c r="K24">
         <v>42.66</v>
       </c>
-      <c r="O24">
-        <v>-0.64990000000000003</v>
-      </c>
     </row>
     <row r="25" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
@@ -3532,9 +3526,6 @@
       <c r="K25">
         <v>42.66</v>
       </c>
-      <c r="O25">
-        <v>-0.69969999999999999</v>
-      </c>
     </row>
     <row r="26" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H26" s="1"/>
@@ -3547,9 +3538,6 @@
       <c r="K26">
         <v>42.66</v>
       </c>
-      <c r="O26">
-        <v>-0.80130000000000001</v>
-      </c>
     </row>
     <row r="27" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H27" s="1"/>
@@ -3562,9 +3550,6 @@
       <c r="K27">
         <v>42.66</v>
       </c>
-      <c r="O27">
-        <v>-0.78710000000000002</v>
-      </c>
     </row>
     <row r="28" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H28" s="1"/>
@@ -3577,9 +3562,6 @@
       <c r="K28">
         <v>42.66</v>
       </c>
-      <c r="O28">
-        <v>-0.71960000000000002</v>
-      </c>
     </row>
     <row r="29" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H29" s="1"/>
@@ -3592,9 +3574,6 @@
       <c r="K29">
         <v>42.66</v>
       </c>
-      <c r="O29">
-        <v>-0.90990000000000004</v>
-      </c>
     </row>
     <row r="30" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H30" s="1"/>
@@ -3607,9 +3586,6 @@
       <c r="K30">
         <v>42.66</v>
       </c>
-      <c r="O30">
-        <v>-0.97109999999999996</v>
-      </c>
     </row>
     <row r="31" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H31" s="1"/>
@@ -3622,9 +3598,6 @@
       <c r="K31">
         <v>42.66</v>
       </c>
-      <c r="O31">
-        <v>-0.98970000000000002</v>
-      </c>
     </row>
     <row r="32" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
@@ -3632,63 +3605,57 @@
         <v>40.581885704420301</v>
       </c>
       <c r="J32">
-        <v>43.762752716241494</v>
+        <v>43.596128420137347</v>
       </c>
       <c r="K32">
         <v>42.66</v>
       </c>
-      <c r="O32">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="33" spans="9:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I33">
         <v>40.379400717021326</v>
       </c>
       <c r="J33">
-        <v>43.121337078600732</v>
+        <v>43.240524423594934</v>
       </c>
       <c r="K33">
         <v>42.66</v>
       </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="9:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I34">
         <v>40.443220964088937</v>
       </c>
       <c r="J34">
-        <v>44.290949408497227</v>
+        <v>43.483368443486484</v>
       </c>
       <c r="K34">
         <v>42.66</v>
       </c>
     </row>
-    <row r="35" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I35">
         <v>40.443672805955259</v>
       </c>
       <c r="J35">
-        <v>46.406778541215033</v>
+        <v>43.484236772437441</v>
       </c>
       <c r="K35">
         <v>42.66</v>
       </c>
     </row>
-    <row r="37" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" t="s">
         <v>25</v>
-      </c>
-      <c r="J37" t="s">
-        <v>26</v>
       </c>
       <c r="K37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I38" s="2">
         <f>(I24-$I$24)/I24</f>
         <v>0</v>
@@ -3701,7 +3668,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="39" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I39" s="2">
         <f t="shared" ref="I39:J39" si="10">(I25-$I$24)/I25</f>
         <v>-1.7406421173819492E-2</v>
@@ -3714,7 +3681,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="40" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I40" s="2">
         <f t="shared" ref="I40:J40" si="11">(I26-$I$24)/I26</f>
         <v>-0.10008540620225891</v>
@@ -3727,7 +3694,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="41" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I41" s="2">
         <f t="shared" ref="I41:J41" si="12">(I27-$I$24)/I27</f>
         <v>-8.98916689619043E-2</v>
@@ -3740,7 +3707,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="42" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I42" s="2">
         <f t="shared" ref="I42:J42" si="13">(I28-$I$24)/I28</f>
         <v>-7.9403134343638354E-2</v>
@@ -3753,7 +3720,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="43" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I43" s="2">
         <f t="shared" ref="I43:J43" si="14">(I29-$I$24)/I29</f>
         <v>-0.1092474661403095</v>
@@ -3766,7 +3733,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="44" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I44" s="2">
         <f t="shared" ref="I44:J44" si="15">(I30-$I$24)/I30</f>
         <v>-0.15018531617362693</v>
@@ -3779,7 +3746,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="45" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I45" s="2">
         <f t="shared" ref="I45:J45" si="16">(I31-$I$24)/I31</f>
         <v>-4.8291852704685376E-2</v>
@@ -3792,40 +3759,40 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="46" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I46" s="2">
         <f t="shared" ref="I46:J46" si="17">(I32-$I$24)/I32</f>
         <v>-5.1207928352953493E-2</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" si="17"/>
-        <v>2.5198431263950855E-2</v>
+        <v>2.1472742054428385E-2</v>
       </c>
       <c r="K46">
         <v>42.66</v>
       </c>
     </row>
-    <row r="47" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I47" s="2">
         <f t="shared" ref="I47:J47" si="18">(I33-$I$24)/I33</f>
         <v>-5.6479275137367883E-2</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" si="18"/>
-        <v>1.069858009643374E-2</v>
+        <v>1.3425471391326538E-2</v>
       </c>
       <c r="K47">
         <v>42.66</v>
       </c>
     </row>
-    <row r="48" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I48" s="2">
         <f t="shared" ref="I48:J48" si="19">(I34-$I$24)/I34</f>
         <v>-5.481212878369477E-2</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="19"/>
-        <v>3.6823536868783514E-2</v>
+        <v>1.8935249796863771E-2</v>
       </c>
       <c r="K48">
         <v>42.66</v>
@@ -3838,7 +3805,7 @@
       </c>
       <c r="J49" s="2">
         <f t="shared" si="20"/>
-        <v>8.0737742609895247E-2</v>
+        <v>1.8954840503487495E-2</v>
       </c>
       <c r="K49">
         <v>42.66</v>

</xml_diff>

<commit_message>
Neural SDE model fit for the write up
</commit_message>
<xml_diff>
--- a/nsde_2021_calibrations/Dynamic_calibration_hedging/Model_market_hedges_comparison.xlsx
+++ b/nsde_2021_calibrations/Dynamic_calibration_hedging/Model_market_hedges_comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s0837263\Desktop\Hedging_strategies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s0837263\to_linux\robust_nsde\nsde_2021_calibrations\Dynamic_calibration_hedging\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>t</t>
   </si>
@@ -105,6 +105,33 @@
   </si>
   <si>
     <t>no vanilla  options traded with required strike (deltas interpolated to -1 at the last re-balancing date)</t>
+  </si>
+  <si>
+    <t>Perfect Hedge Lookback</t>
+  </si>
+  <si>
+    <t>Perfect Hedge Straddle</t>
+  </si>
+  <si>
+    <t>Price Prediction (Straddle Hedge based)</t>
+  </si>
+  <si>
+    <t>Price Prediction (Lookback Hedge based)</t>
+  </si>
+  <si>
+    <t>Price Realised</t>
+  </si>
+  <si>
+    <t>Prediction Average</t>
+  </si>
+  <si>
+    <t>Prediction (Average Basket and Lookback) Error</t>
+  </si>
+  <si>
+    <t>Price Prediction (Market Straddle Delta)</t>
+  </si>
+  <si>
+    <t>Price Prediction (Model Straddle Delta)</t>
   </si>
 </sst>
 </file>
@@ -1187,6 +1214,1077 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Realised</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> and predicted prices </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price Prediction (Lookback Hedge based)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$22:$S$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>765.91399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>794.91873750320758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>808.65314100216551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>814.4475161071648</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>818.81323529489202</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>817.46882326592822</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>807.53284111736627</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>814.09505046920879</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>824.73203170593808</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>823.51450529447641</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>828.99464416532646</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9A0B-4209-9C9F-1A02BD99F3D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price Prediction (Straddle Hedge based)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$22:$T$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>765.91399999999987</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>797.70053832619624</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>793.50074183852053</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>802.27554623764877</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>809.01727175426083</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>803.23220219984466</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>793.09950096392436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>816.44170166468575</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>822.00028586877863</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>817.70392992489099</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>826.97577151279256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9A0B-4209-9C9F-1A02BD99F3D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$U$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price Realised</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$22:$U$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>765.91399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>799.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800.11400000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>807.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>813.45399999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>809.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>801.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>819.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>824.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>820.43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>829.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9A0B-4209-9C9F-1A02BD99F3D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="622473624"/>
+        <c:axId val="622474280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="622473624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="622474280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="622474280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="622473624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Price Prediction Market/Model</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price Prediction (Market Straddle Delta)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$22:$X$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>765.91399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>814.36442688573084</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>802.71164810320226</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>810.03525523585859</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>815.32607118712701</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>809.99399420984696</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>801.40681048488716</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>820.1673147534442</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>825.57120686645715</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>821.02847878721127</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>830.43336844348642</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94E3-4D57-9FDD-6516764443C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price Prediction (Model Straddle Delta)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$22:$Y$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>765.91399999999987</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>798.48900892166535</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>794.14201556790408</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>802.871423191654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>809.53766639175933</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>803.76205780797898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>793.67913754414053</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>816.90017361205537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>822.43004088602652</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>818.12566607762085</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>827.39322096408887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-94E3-4D57-9FDD-6516764443C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price Realised</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$22:$Z$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>765.91399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>799.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800.11400000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>807.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>813.45399999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>809.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>801.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>819.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>824.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>820.43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>829.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-94E3-4D57-9FDD-6516764443C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="695847992"/>
+        <c:axId val="695849304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="695847992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="695849304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="695849304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="695847992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1267,6 +2365,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2273,20 +3451,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>242887</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1052512</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1004887</xdr:colOff>
+      <xdr:colOff>414337</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2330,6 +4514,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2109787</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1585912</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2601,10 +4845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:U49"/>
+  <dimension ref="A2:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,12 +4867,20 @@
     <col min="14" max="14" width="17.28515625" customWidth="1"/>
     <col min="15" max="15" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.28515625" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" customWidth="1"/>
+    <col min="19" max="19" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.28515625" customWidth="1"/>
+    <col min="23" max="23" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>-6.4100000000000004E-2</v>
+      </c>
+    </row>
     <row r="4" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
@@ -2708,7 +4960,7 @@
         <v>29.27</v>
       </c>
       <c r="L5">
-        <v>-6.4100000000000004E-2</v>
+        <v>-7.6410000000000006E-2</v>
       </c>
       <c r="M5">
         <v>0.10569248108238501</v>
@@ -2718,26 +4970,26 @@
       </c>
       <c r="P5">
         <f>-L5*H5</f>
-        <v>49.095087400000004</v>
+        <v>58.523488740000005</v>
       </c>
       <c r="Q5">
         <f>-O5*H5</f>
         <v>-236.20787759999999</v>
       </c>
       <c r="R5">
-        <f t="shared" ref="R5:R16" si="0">I5+P5+L5*H5</f>
-        <v>42.660000000000004</v>
+        <f>I5+P5+L5*H5</f>
+        <v>42.66</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S16" si="1">J5+Q5+O5*H5</f>
+        <f t="shared" ref="S5:S16" si="0">J5+Q5+O5*H5</f>
         <v>29.27000000000001</v>
       </c>
       <c r="T5" s="2">
-        <f t="shared" ref="T5:T16" si="2">(R5-$R$5)/$R$5</f>
+        <f t="shared" ref="T5:T16" si="1">(R5-$R$5)/$R$5</f>
         <v>0</v>
       </c>
       <c r="U5" s="2">
-        <f t="shared" ref="U5:U16" si="3">(S5-$S$5)/$S$5</f>
+        <f t="shared" ref="U5:U16" si="2">(S5-$S$5)/$S$5</f>
         <v>0</v>
       </c>
     </row>
@@ -2766,8 +5018,8 @@
         <v>20.54</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:K16" si="4">L6-L5</f>
-        <v>-0.46439999999999998</v>
+        <f>L6-L5</f>
+        <v>-0.45208999999999999</v>
       </c>
       <c r="L6">
         <v>-0.52849999999999997</v>
@@ -2783,27 +5035,27 @@
         <v>0.3453</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6:P16" si="5">P5*E6-K6*H6</f>
-        <v>420.5614412151001</v>
+        <f t="shared" ref="P6:P16" si="3">P5*E6-K6*H6</f>
+        <v>420.14473450539469</v>
       </c>
       <c r="Q6">
-        <f t="shared" ref="Q6:Q16" si="6">Q5*E6-N6*H6</f>
+        <f t="shared" ref="Q6:Q16" si="4">Q5*E6-N6*H6</f>
         <v>-265.75544005985762</v>
       </c>
       <c r="R6">
+        <f>I6+P6+L6*H6</f>
+        <v>41.513439505394729</v>
+      </c>
+      <c r="S6">
         <f t="shared" si="0"/>
-        <v>41.930146215100137</v>
-      </c>
-      <c r="S6">
+        <v>30.97967094014237</v>
+      </c>
+      <c r="T6" s="2">
         <f t="shared" si="1"/>
-        <v>30.97967094014237</v>
-      </c>
-      <c r="T6" s="2">
+        <v>-2.6876711078416972E-2</v>
+      </c>
+      <c r="U6" s="2">
         <f t="shared" si="2"/>
-        <v>-1.7108621305669626E-2</v>
-      </c>
-      <c r="U6" s="2">
-        <f t="shared" si="3"/>
         <v>5.8410349851122617E-2</v>
       </c>
     </row>
@@ -2812,14 +5064,14 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E16" si="7">EXP(0.05*(F7-F6)/365)</f>
+        <f t="shared" ref="E7:E16" si="5">EXP(0.05*(F7-F6)/365)</f>
         <v>1.0001369956844217</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G16" si="8">H7-H6</f>
+        <f t="shared" ref="G7:G16" si="6">H7-H6</f>
         <v>0.24400000000002819</v>
       </c>
       <c r="H7">
@@ -2832,7 +5084,7 @@
         <v>16.190000000000001</v>
       </c>
       <c r="K7">
-        <f t="shared" si="4"/>
+        <f>L7-L6</f>
         <v>-0.12140000000000006</v>
       </c>
       <c r="L7">
@@ -2842,34 +5094,34 @@
         <v>-0.72825836118487397</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N15" si="9">O7-O6</f>
+        <f t="shared" ref="N7:N15" si="7">O7-O6</f>
         <v>-4.1700000000000015E-2</v>
       </c>
       <c r="O7">
         <v>0.30359999999999998</v>
       </c>
       <c r="P7">
-        <f t="shared" si="5"/>
-        <v>517.75289591758087</v>
+        <f t="shared" si="3"/>
+        <v>517.33613212085447</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-232.42709360825739</v>
       </c>
       <c r="R7">
+        <f>I7+P7+L7*H7</f>
+        <v>38.3620435208544</v>
+      </c>
+      <c r="S7">
         <f t="shared" si="0"/>
-        <v>38.778807317580799</v>
-      </c>
-      <c r="S7">
+        <v>26.67751679174259</v>
+      </c>
+      <c r="T7" s="2">
         <f t="shared" si="1"/>
-        <v>26.67751679174259</v>
-      </c>
-      <c r="T7" s="2">
+        <v>-0.10074909702638531</v>
+      </c>
+      <c r="U7" s="2">
         <f t="shared" si="2"/>
-        <v>-9.0979669067491886E-2</v>
-      </c>
-      <c r="U7" s="2">
-        <f t="shared" si="3"/>
         <v>-8.8571342953789503E-2</v>
       </c>
     </row>
@@ -2878,14 +5130,14 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0004110433592888</v>
       </c>
       <c r="F8">
         <v>5</v>
       </c>
       <c r="G8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>7.7859999999999445</v>
       </c>
       <c r="H8">
@@ -2898,7 +5150,7 @@
         <v>14.29</v>
       </c>
       <c r="K8">
-        <f t="shared" si="4"/>
+        <f>L8-L7</f>
         <v>-4.9799999999999955E-2</v>
       </c>
       <c r="L8">
@@ -2908,34 +5160,34 @@
         <v>-0.78327956506084595</v>
       </c>
       <c r="N8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3.6100000000000021E-2</v>
       </c>
       <c r="O8">
         <v>0.3397</v>
       </c>
       <c r="P8">
-        <f t="shared" si="5"/>
-        <v>558.19913480720027</v>
+        <f t="shared" si="3"/>
+        <v>557.78219970248279</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-261.68782122160388</v>
       </c>
       <c r="R8">
+        <f>I8+P8+L8*H8</f>
+        <v>38.724569702482881</v>
+      </c>
+      <c r="S8">
         <f t="shared" si="0"/>
-        <v>39.141504807200363</v>
-      </c>
-      <c r="S8">
+        <v>27.045808778396093</v>
+      </c>
+      <c r="T8" s="2">
         <f t="shared" si="1"/>
-        <v>27.045808778396093</v>
-      </c>
-      <c r="T8" s="2">
+        <v>-9.2251061826467778E-2</v>
+      </c>
+      <c r="U8" s="2">
         <f t="shared" si="2"/>
-        <v>-8.247761820908675E-2</v>
-      </c>
-      <c r="U8" s="2">
-        <f t="shared" si="3"/>
         <v>-7.5988767393369183E-2</v>
       </c>
     </row>
@@ -2944,14 +5196,14 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F9">
         <v>6</v>
       </c>
       <c r="G9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5.5539999999999736</v>
       </c>
       <c r="H9">
@@ -2964,7 +5216,7 @@
         <v>12.95</v>
       </c>
       <c r="K9">
-        <f t="shared" si="4"/>
+        <f>L9-L8</f>
         <v>-0.10160000000000002</v>
       </c>
       <c r="L9">
@@ -2974,34 +5226,34 @@
         <v>-0.85392030114671702</v>
       </c>
       <c r="N9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>-2.0000000000000018E-2</v>
       </c>
       <c r="O9">
         <v>0.31969999999999998</v>
       </c>
       <c r="P9">
-        <f t="shared" si="5"/>
-        <v>640.9225320797168</v>
+        <f t="shared" si="3"/>
+        <v>640.50553985668921</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-245.45459132377695</v>
       </c>
       <c r="R9">
+        <f>I9+P9+L9*H9</f>
+        <v>39.104849656689225</v>
+      </c>
+      <c r="S9">
         <f t="shared" si="0"/>
-        <v>39.521841879716817</v>
-      </c>
-      <c r="S9">
+        <v>27.556652476223036</v>
+      </c>
+      <c r="T9" s="2">
         <f t="shared" si="1"/>
-        <v>27.556652476223036</v>
-      </c>
-      <c r="T9" s="2">
+        <v>-8.3336857555339233E-2</v>
+      </c>
+      <c r="U9" s="2">
         <f t="shared" si="2"/>
-        <v>-7.3562075018358805E-2</v>
-      </c>
-      <c r="U9" s="2">
-        <f t="shared" si="3"/>
         <v>-5.8535959131430608E-2</v>
       </c>
     </row>
@@ -3010,14 +5262,14 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F10">
         <v>7</v>
       </c>
       <c r="G10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>-4.3539999999999281</v>
       </c>
       <c r="H10">
@@ -3030,7 +5282,7 @@
         <v>12.8</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <f>L10-L9</f>
         <v>1.419999999999999E-2</v>
       </c>
       <c r="L10">
@@ -3040,35 +5292,34 @@
         <v>-0.86229317908810799</v>
       </c>
       <c r="N10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7.3300000000000032E-2</v>
       </c>
       <c r="O10">
-        <f>0.393</f>
         <v>0.39300000000000002</v>
       </c>
       <c r="P10">
-        <f t="shared" si="5"/>
-        <v>629.52111570066029</v>
+        <f t="shared" si="3"/>
+        <v>629.10406635149775</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-304.79524754350984</v>
       </c>
       <c r="R10">
+        <f>I10+P10+L10*H10</f>
+        <v>38.041456351497686</v>
+      </c>
+      <c r="S10">
         <f t="shared" si="0"/>
-        <v>38.458505700660226</v>
-      </c>
-      <c r="S10">
+        <v>25.981052456490204</v>
+      </c>
+      <c r="T10" s="2">
         <f t="shared" si="1"/>
-        <v>25.981052456490204</v>
-      </c>
-      <c r="T10" s="2">
+        <v>-0.1082640330169318</v>
+      </c>
+      <c r="U10" s="2">
         <f t="shared" si="2"/>
-        <v>-9.848791137692868E-2</v>
-      </c>
-      <c r="U10" s="2">
-        <f t="shared" si="3"/>
         <v>-0.11236581973043407</v>
       </c>
     </row>
@@ -3077,14 +5328,14 @@
         <v>6</v>
       </c>
       <c r="E11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F11">
         <v>8</v>
       </c>
       <c r="G11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>-7.6800000000000637</v>
       </c>
       <c r="H11">
@@ -3097,7 +5348,7 @@
         <v>15.62</v>
       </c>
       <c r="K11">
-        <f t="shared" si="4"/>
+        <f>L11-L10</f>
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="L11">
@@ -3107,35 +5358,34 @@
         <v>-0.86779167973132199</v>
       </c>
       <c r="N11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.18430000000000002</v>
       </c>
       <c r="O11">
-        <f>0.5773</f>
         <v>0.57730000000000004</v>
       </c>
       <c r="P11">
-        <f t="shared" si="5"/>
-        <v>575.51150737676357</v>
+        <f t="shared" si="3"/>
+        <v>575.09440089364</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-452.53870917705558</v>
       </c>
       <c r="R11">
+        <f>I11+P11+L11*H11</f>
+        <v>36.672568893640005</v>
+      </c>
+      <c r="S11">
         <f t="shared" si="0"/>
-        <v>37.08967537676358</v>
-      </c>
-      <c r="S11">
+        <v>25.741056822944415</v>
+      </c>
+      <c r="T11" s="2">
         <f t="shared" si="1"/>
-        <v>25.741056822944415</v>
-      </c>
-      <c r="T11" s="2">
+        <v>-0.14035234660947005</v>
+      </c>
+      <c r="U11" s="2">
         <f t="shared" si="2"/>
-        <v>-0.13057488568299164</v>
-      </c>
-      <c r="U11" s="2">
-        <f t="shared" si="3"/>
         <v>-0.1205651922465184</v>
       </c>
     </row>
@@ -3144,14 +5394,14 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F12">
         <v>9</v>
       </c>
       <c r="G12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>17.639999999999986</v>
       </c>
       <c r="H12">
@@ -3164,7 +5414,7 @@
         <v>10.85</v>
       </c>
       <c r="K12">
-        <f t="shared" si="4"/>
+        <f>L12-L11</f>
         <v>-0.19030000000000002</v>
       </c>
       <c r="L12">
@@ -3175,34 +5425,34 @@
         <v>-0.9</v>
       </c>
       <c r="N12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>-0.21020000000000005</v>
       </c>
       <c r="O12">
         <v>0.36709999999999998</v>
       </c>
       <c r="P12">
-        <f t="shared" si="5"/>
-        <v>731.45746796960918</v>
+        <f t="shared" si="3"/>
+        <v>731.04030434469757</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-280.43429302724655</v>
       </c>
       <c r="R12">
+        <f>I12+P12+L12*H12</f>
+        <v>40.277610344697564</v>
+      </c>
+      <c r="S12">
         <f t="shared" si="0"/>
-        <v>40.694773969609173</v>
-      </c>
-      <c r="S12">
+        <v>31.092632972753449</v>
+      </c>
+      <c r="T12" s="2">
         <f t="shared" si="1"/>
-        <v>31.092632972753449</v>
-      </c>
-      <c r="T12" s="2">
+        <v>-5.5845983481069686E-2</v>
+      </c>
+      <c r="U12" s="2">
         <f t="shared" si="2"/>
-        <v>-4.6067183084642062E-2</v>
-      </c>
-      <c r="U12" s="2">
-        <f t="shared" si="3"/>
         <v>6.2269660838860215E-2</v>
       </c>
     </row>
@@ -3211,14 +5461,14 @@
         <v>8</v>
       </c>
       <c r="E13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0004110433592888</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5.5100000000001046</v>
       </c>
       <c r="H13">
@@ -3231,7 +5481,7 @@
         <v>7.05</v>
       </c>
       <c r="K13">
-        <f t="shared" si="4"/>
+        <f>L13-L12</f>
         <v>-6.1199999999999921E-2</v>
       </c>
       <c r="L13">
@@ -3241,34 +5491,34 @@
         <v>-0.93500000000000005</v>
       </c>
       <c r="N13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6.4400000000000013E-2</v>
       </c>
       <c r="O13">
         <v>0.43149999999999999</v>
       </c>
       <c r="P13">
-        <f t="shared" si="5"/>
-        <v>782.22181270442024</v>
+        <f t="shared" si="3"/>
+        <v>781.80447760717084</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-333.65187168111225</v>
       </c>
       <c r="R13">
+        <f>I13+P13+L13*H13</f>
+        <v>40.164550607170895</v>
+      </c>
+      <c r="S13">
         <f t="shared" si="0"/>
-        <v>40.581885704420301</v>
-      </c>
-      <c r="S13">
+        <v>29.200083318887778</v>
+      </c>
+      <c r="T13" s="2">
         <f t="shared" si="1"/>
-        <v>29.200083318887778</v>
-      </c>
-      <c r="T13" s="2">
+        <v>-5.8496235181179128E-2</v>
+      </c>
+      <c r="U13" s="2">
         <f t="shared" si="2"/>
-        <v>-4.8713415273785796E-2</v>
-      </c>
-      <c r="U13" s="2">
-        <f t="shared" si="3"/>
         <v>-2.3886805982997082E-3</v>
       </c>
     </row>
@@ -3277,14 +5527,14 @@
         <v>9</v>
       </c>
       <c r="E14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
       <c r="G14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>-4.1400000000001</v>
       </c>
       <c r="H14">
@@ -3297,7 +5547,7 @@
         <v>7.06</v>
       </c>
       <c r="K14">
-        <f t="shared" si="4"/>
+        <f>L14-L13</f>
         <v>-1.8600000000000061E-2</v>
       </c>
       <c r="L14">
@@ -3307,34 +5557,34 @@
         <v>-0.97</v>
       </c>
       <c r="N14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.18189999999999995</v>
       </c>
       <c r="O14">
         <v>0.61339999999999995</v>
       </c>
       <c r="P14">
-        <f t="shared" si="5"/>
-        <v>797.58897171702131</v>
+        <f t="shared" si="3"/>
+        <v>797.17157944666462</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-482.93379754763174</v>
       </c>
       <c r="R14">
+        <f>I14+P14+L14*H14</f>
+        <v>39.96200844666464</v>
+      </c>
+      <c r="S14">
         <f t="shared" si="0"/>
-        <v>40.379400717021326</v>
-      </c>
-      <c r="S14">
+        <v>27.37796445236819</v>
+      </c>
+      <c r="T14" s="2">
         <f t="shared" si="1"/>
-        <v>27.37796445236819</v>
-      </c>
-      <c r="T14" s="2">
+        <v>-6.3244058915502971E-2</v>
+      </c>
+      <c r="U14" s="2">
         <f t="shared" si="2"/>
-        <v>-5.3459898804000872E-2</v>
-      </c>
-      <c r="U14" s="2">
-        <f t="shared" si="3"/>
         <v>-6.4640777165419203E-2</v>
       </c>
     </row>
@@ -3343,14 +5593,14 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F15">
         <v>14</v>
       </c>
       <c r="G15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9.1800000000000637</v>
       </c>
       <c r="H15">
@@ -3363,7 +5613,7 @@
         <v>3.69</v>
       </c>
       <c r="K15">
-        <f t="shared" si="4"/>
+        <f>L15-L14</f>
         <v>-1.0299999999999976E-2</v>
       </c>
       <c r="L15">
@@ -3373,34 +5623,34 @@
         <v>-1</v>
       </c>
       <c r="N15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>-0.12129999999999996</v>
       </c>
       <c r="O15">
         <v>0.49209999999999998</v>
       </c>
       <c r="P15">
-        <f t="shared" si="5"/>
-        <v>806.24322096408889</v>
+        <f t="shared" si="3"/>
+        <v>805.82577151279247</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-382.36826439375716</v>
       </c>
       <c r="R15">
+        <f>I15+P15+L15*H15</f>
+        <v>40.025771512792403</v>
+      </c>
+      <c r="S15">
         <f t="shared" si="0"/>
-        <v>40.443220964088937</v>
-      </c>
-      <c r="S15">
+        <v>29.572816606242839</v>
+      </c>
+      <c r="T15" s="2">
         <f t="shared" si="1"/>
-        <v>29.572816606242839</v>
-      </c>
-      <c r="T15" s="2">
+        <v>-6.1749378509320059E-2</v>
+      </c>
+      <c r="U15" s="2">
         <f t="shared" si="2"/>
-        <v>-5.1963878010104707E-2</v>
-      </c>
-      <c r="U15" s="2">
-        <f t="shared" si="3"/>
         <v>1.0345630551514461E-2</v>
       </c>
     </row>
@@ -3409,14 +5659,14 @@
         <v>11</v>
       </c>
       <c r="E16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F16">
         <v>15</v>
       </c>
       <c r="G16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>16.110000000000014</v>
       </c>
       <c r="H16">
@@ -3429,7 +5679,7 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="4"/>
+        <f>L16-L15</f>
         <v>1</v>
       </c>
       <c r="L16">
@@ -3446,31 +5696,34 @@
         <v>0</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" si="5"/>
-        <v>-39.366327194044743</v>
+        <f t="shared" si="3"/>
+        <v>-39.783833834114489</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>33.758164804161083</v>
       </c>
       <c r="R16">
+        <f>I16+P16+L16*H16</f>
+        <v>40.026166165885513</v>
+      </c>
+      <c r="S16">
         <f t="shared" si="0"/>
-        <v>40.443672805955259</v>
-      </c>
-      <c r="S16">
+        <v>33.758164804161083</v>
+      </c>
+      <c r="T16" s="2">
         <f t="shared" si="1"/>
-        <v>33.758164804161083</v>
-      </c>
-      <c r="T16" s="2">
+        <v>-6.1740127381961642E-2</v>
+      </c>
+      <c r="U16" s="2">
         <f t="shared" si="2"/>
-        <v>-5.1953286311409851E-2</v>
-      </c>
-      <c r="U16" s="2">
-        <f t="shared" si="3"/>
         <v>0.1533366861688101</v>
       </c>
     </row>
-    <row r="17" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>845.72</v>
+      </c>
       <c r="P17" s="4" t="s">
         <v>18</v>
       </c>
@@ -3478,20 +5731,89 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:26" x14ac:dyDescent="0.25">
       <c r="K18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="21" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="S21" s="2"/>
+    <row r="21" spans="8:26" x14ac:dyDescent="0.25">
+      <c r="P21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>27</v>
+      </c>
+      <c r="R21" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T21" t="s">
+        <v>29</v>
+      </c>
+      <c r="U21" t="s">
+        <v>31</v>
+      </c>
+      <c r="V21" t="s">
+        <v>32</v>
+      </c>
+      <c r="W21" t="s">
+        <v>33</v>
+      </c>
+      <c r="X21" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="22" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H22" s="1"/>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R22">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S22">
+        <f>(Q22-Q5-J5)/O5</f>
+        <v>765.91399999999999</v>
+      </c>
+      <c r="T22">
+        <f>(R22-P5-I5)/L5</f>
+        <v>765.91399999999987</v>
+      </c>
+      <c r="U22">
+        <v>765.91399999999999</v>
+      </c>
+      <c r="V22">
+        <f>(S22+T22)/2</f>
+        <v>765.91399999999999</v>
+      </c>
+      <c r="W22" s="2">
+        <f>(V22-U22)/V22</f>
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>765.91399999999999</v>
+      </c>
+      <c r="Y22">
+        <v>765.91399999999987</v>
+      </c>
+      <c r="Z22">
+        <v>765.91399999999999</v>
+      </c>
     </row>
-    <row r="23" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H23" s="1"/>
       <c r="I23" t="s">
         <v>20</v>
@@ -3502,8 +5824,45 @@
       <c r="K23" t="s">
         <v>22</v>
       </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R23">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S23">
+        <f>(Q23-Q6-J6)/O6</f>
+        <v>794.91873750320758</v>
+      </c>
+      <c r="T23">
+        <f>(R23-P6-I6)/L6</f>
+        <v>797.70053832619624</v>
+      </c>
+      <c r="U23">
+        <v>799.87</v>
+      </c>
+      <c r="V23">
+        <f t="shared" ref="V23:V32" si="8">(S23+T23)/2</f>
+        <v>796.30963791470185</v>
+      </c>
+      <c r="W23" s="2">
+        <f t="shared" ref="W23:W32" si="9">(V23-U23)/V23</f>
+        <v>-4.4710774751159383E-3</v>
+      </c>
+      <c r="X23">
+        <v>814.36442688573084</v>
+      </c>
+      <c r="Y23">
+        <v>798.48900892166535</v>
+      </c>
+      <c r="Z23">
+        <v>799.87</v>
+      </c>
     </row>
-    <row r="24" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H24" s="1"/>
       <c r="I24">
         <v>42.660000000000004</v>
@@ -3514,8 +5873,45 @@
       <c r="K24">
         <v>42.66</v>
       </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+      <c r="Q24">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R24">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S24">
+        <f t="shared" ref="S24:S33" si="10">(Q24-Q7-J7)/O7</f>
+        <v>808.65314100216551</v>
+      </c>
+      <c r="T24">
+        <f>(R24-P7-I7)/L7</f>
+        <v>793.50074183852053</v>
+      </c>
+      <c r="U24">
+        <v>800.11400000000003</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="8"/>
+        <v>801.07694142034302</v>
+      </c>
+      <c r="W24" s="2">
+        <f t="shared" si="9"/>
+        <v>1.2020585920693842E-3</v>
+      </c>
+      <c r="X24">
+        <v>802.71164810320226</v>
+      </c>
+      <c r="Y24">
+        <v>794.14201556790408</v>
+      </c>
+      <c r="Z24">
+        <v>800.11400000000003</v>
+      </c>
     </row>
-    <row r="25" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
       <c r="I25">
         <v>41.930146215100137</v>
@@ -3526,8 +5922,45 @@
       <c r="K25">
         <v>42.66</v>
       </c>
+      <c r="P25">
+        <v>5</v>
+      </c>
+      <c r="Q25">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R25">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="10"/>
+        <v>814.4475161071648</v>
+      </c>
+      <c r="T25">
+        <f>(R25-P8-I8)/L8</f>
+        <v>802.27554623764877</v>
+      </c>
+      <c r="U25">
+        <v>807.9</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="8"/>
+        <v>808.36153117240679</v>
+      </c>
+      <c r="W25" s="2">
+        <f t="shared" si="9"/>
+        <v>5.7094648199973886E-4</v>
+      </c>
+      <c r="X25">
+        <v>810.03525523585859</v>
+      </c>
+      <c r="Y25">
+        <v>802.871423191654</v>
+      </c>
+      <c r="Z25">
+        <v>807.9</v>
+      </c>
     </row>
-    <row r="26" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H26" s="1"/>
       <c r="I26">
         <v>38.778807317580799</v>
@@ -3538,8 +5971,45 @@
       <c r="K26">
         <v>42.66</v>
       </c>
+      <c r="P26">
+        <v>6</v>
+      </c>
+      <c r="Q26">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R26">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="10"/>
+        <v>818.81323529489202</v>
+      </c>
+      <c r="T26">
+        <f>(R26-P9-I9)/L9</f>
+        <v>809.01727175426083</v>
+      </c>
+      <c r="U26">
+        <v>813.45399999999995</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="8"/>
+        <v>813.91525352457643</v>
+      </c>
+      <c r="W26" s="2">
+        <f t="shared" si="9"/>
+        <v>5.6670952237234339E-4</v>
+      </c>
+      <c r="X26">
+        <v>815.32607118712701</v>
+      </c>
+      <c r="Y26">
+        <v>809.53766639175933</v>
+      </c>
+      <c r="Z26">
+        <v>813.45399999999995</v>
+      </c>
     </row>
-    <row r="27" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H27" s="1"/>
       <c r="I27">
         <v>39.141504807200363</v>
@@ -3550,8 +6020,45 @@
       <c r="K27">
         <v>42.66</v>
       </c>
+      <c r="P27">
+        <v>7</v>
+      </c>
+      <c r="Q27">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R27">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="10"/>
+        <v>817.46882326592822</v>
+      </c>
+      <c r="T27">
+        <f>(R27-P10-I10)/L10</f>
+        <v>803.23220219984466</v>
+      </c>
+      <c r="U27">
+        <v>809.1</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="8"/>
+        <v>810.3505127328865</v>
+      </c>
+      <c r="W27" s="2">
+        <f t="shared" si="9"/>
+        <v>1.5431750992162083E-3</v>
+      </c>
+      <c r="X27">
+        <v>809.99399420984696</v>
+      </c>
+      <c r="Y27">
+        <v>803.76205780797898</v>
+      </c>
+      <c r="Z27">
+        <v>809.1</v>
+      </c>
     </row>
-    <row r="28" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H28" s="1"/>
       <c r="I28">
         <v>39.521841879716817</v>
@@ -3562,8 +6069,45 @@
       <c r="K28">
         <v>42.66</v>
       </c>
+      <c r="P28">
+        <v>8</v>
+      </c>
+      <c r="Q28">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R28">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="10"/>
+        <v>807.53284111736627</v>
+      </c>
+      <c r="T28">
+        <f>(R28-P11-I11)/L11</f>
+        <v>793.09950096392436</v>
+      </c>
+      <c r="U28">
+        <v>801.42</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="8"/>
+        <v>800.31617104064526</v>
+      </c>
+      <c r="W28" s="2">
+        <f t="shared" si="9"/>
+        <v>-1.3792411040744058E-3</v>
+      </c>
+      <c r="X28">
+        <v>801.40681048488716</v>
+      </c>
+      <c r="Y28">
+        <v>793.67913754414053</v>
+      </c>
+      <c r="Z28">
+        <v>801.42</v>
+      </c>
     </row>
-    <row r="29" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H29" s="1"/>
       <c r="I29">
         <v>38.458505700660226</v>
@@ -3574,8 +6118,45 @@
       <c r="K29">
         <v>42.66</v>
       </c>
+      <c r="P29">
+        <v>9</v>
+      </c>
+      <c r="Q29">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R29">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="10"/>
+        <v>814.09505046920879</v>
+      </c>
+      <c r="T29">
+        <f>(R29-P12-I12)/L12</f>
+        <v>816.44170166468575</v>
+      </c>
+      <c r="U29">
+        <v>819.06</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="8"/>
+        <v>815.26837606694721</v>
+      </c>
+      <c r="W29" s="2">
+        <f t="shared" si="9"/>
+        <v>-4.6507678261046362E-3</v>
+      </c>
+      <c r="X29">
+        <v>820.1673147534442</v>
+      </c>
+      <c r="Y29">
+        <v>816.90017361205537</v>
+      </c>
+      <c r="Z29">
+        <v>819.06</v>
+      </c>
     </row>
-    <row r="30" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H30" s="1"/>
       <c r="I30">
         <v>37.08967537676358</v>
@@ -3586,8 +6167,45 @@
       <c r="K30">
         <v>42.66</v>
       </c>
+      <c r="P30">
+        <v>12</v>
+      </c>
+      <c r="Q30">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R30">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="10"/>
+        <v>824.73203170593808</v>
+      </c>
+      <c r="T30">
+        <f>(R30-P13-I13)/L13</f>
+        <v>822.00028586877863</v>
+      </c>
+      <c r="U30">
+        <v>824.57</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="8"/>
+        <v>823.36615878735836</v>
+      </c>
+      <c r="W30" s="2">
+        <f t="shared" si="9"/>
+        <v>-1.4620970266918563E-3</v>
+      </c>
+      <c r="X30">
+        <v>825.57120686645715</v>
+      </c>
+      <c r="Y30">
+        <v>822.43004088602652</v>
+      </c>
+      <c r="Z30">
+        <v>824.57</v>
+      </c>
     </row>
-    <row r="31" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H31" s="1"/>
       <c r="I31">
         <v>40.694773969609173</v>
@@ -3598,8 +6216,45 @@
       <c r="K31">
         <v>42.66</v>
       </c>
+      <c r="P31">
+        <v>13</v>
+      </c>
+      <c r="Q31">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R31">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="10"/>
+        <v>823.51450529447641</v>
+      </c>
+      <c r="T31">
+        <f>(R31-P14-I14)/L14</f>
+        <v>817.70392992489099</v>
+      </c>
+      <c r="U31">
+        <v>820.43</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="8"/>
+        <v>820.6092176096837</v>
+      </c>
+      <c r="W31" s="2">
+        <f t="shared" si="9"/>
+        <v>2.1839580379779503E-4</v>
+      </c>
+      <c r="X31">
+        <v>821.02847878721127</v>
+      </c>
+      <c r="Y31">
+        <v>818.12566607762085</v>
+      </c>
+      <c r="Z31">
+        <v>820.43</v>
+      </c>
     </row>
-    <row r="32" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
       <c r="I32">
         <v>40.581885704420301</v>
@@ -3610,8 +6265,45 @@
       <c r="K32">
         <v>42.66</v>
       </c>
+      <c r="P32">
+        <v>14</v>
+      </c>
+      <c r="Q32">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R32">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="10"/>
+        <v>828.99464416532646</v>
+      </c>
+      <c r="T32">
+        <f>(R32-P15-I15)/L15</f>
+        <v>826.97577151279256</v>
+      </c>
+      <c r="U32">
+        <v>829.61</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="8"/>
+        <v>827.98520783905951</v>
+      </c>
+      <c r="W32" s="2">
+        <f t="shared" si="9"/>
+        <v>-1.9623444302598238E-3</v>
+      </c>
+      <c r="X32">
+        <v>830.43336844348642</v>
+      </c>
+      <c r="Y32">
+        <v>827.39322096408887</v>
+      </c>
+      <c r="Z32">
+        <v>829.61</v>
+      </c>
     </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I33">
         <v>40.379400717021326</v>
       </c>
@@ -3621,8 +6313,38 @@
       <c r="K33">
         <v>42.66</v>
       </c>
+      <c r="P33">
+        <v>15</v>
+      </c>
+      <c r="Q33">
+        <v>29.27000000000001</v>
+      </c>
+      <c r="R33">
+        <v>42.660000000000004</v>
+      </c>
+      <c r="S33" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T33" t="e">
+        <f>(R33-P16-I16)/L16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U33">
+        <v>845.72</v>
+      </c>
+      <c r="V33" t="e">
+        <f>(S33+T33)/2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X33" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z33">
+        <v>845.72</v>
+      </c>
     </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I34">
         <v>40.443220964088937</v>
       </c>
@@ -3633,7 +6355,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I35">
         <v>40.443672805955259</v>
       </c>
@@ -3644,7 +6366,7 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
         <v>24</v>
       </c>
@@ -3655,7 +6377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I38" s="2">
         <f>(I24-$I$24)/I24</f>
         <v>0</v>
@@ -3668,130 +6390,130 @@
         <v>42.66</v>
       </c>
     </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I39" s="2">
-        <f t="shared" ref="I39:J39" si="10">(I25-$I$24)/I25</f>
+        <f t="shared" ref="I39:J39" si="11">(I25-$I$24)/I25</f>
         <v>-1.7406421173819492E-2</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10524402324042351</v>
       </c>
       <c r="K39">
         <v>42.66</v>
       </c>
     </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I40" s="2">
-        <f t="shared" ref="I40:J40" si="11">(I26-$I$24)/I26</f>
+        <f t="shared" ref="I40:J40" si="12">(I26-$I$24)/I26</f>
         <v>-0.10008540620225891</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4.2462048528134899E-2</v>
       </c>
       <c r="K40">
         <v>42.66</v>
       </c>
     </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I41" s="2">
-        <f t="shared" ref="I41:J41" si="12">(I27-$I$24)/I27</f>
+        <f t="shared" ref="I41:J41" si="13">(I27-$I$24)/I27</f>
         <v>-8.98916689619043E-2</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.7726311956580293E-2</v>
       </c>
       <c r="K41">
         <v>42.66</v>
       </c>
     </row>
-    <row r="42" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I42" s="2">
-        <f t="shared" ref="I42:J42" si="13">(I28-$I$24)/I28</f>
+        <f t="shared" ref="I42:J42" si="14">(I28-$I$24)/I28</f>
         <v>-7.9403134343638354E-2</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.6119524942513158E-2</v>
       </c>
       <c r="K42">
         <v>42.66</v>
       </c>
     </row>
-    <row r="43" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I43" s="2">
-        <f t="shared" ref="I43:J43" si="14">(I29-$I$24)/I29</f>
+        <f t="shared" ref="I43:J43" si="15">(I29-$I$24)/I29</f>
         <v>-0.1092474661403095</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7749698339217756E-2</v>
       </c>
       <c r="K43">
         <v>42.66</v>
       </c>
     </row>
-    <row r="44" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I44" s="2">
-        <f t="shared" ref="I44:J44" si="15">(I30-$I$24)/I30</f>
+        <f t="shared" ref="I44:J44" si="16">(I30-$I$24)/I30</f>
         <v>-0.15018531617362693</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.6837372746244225E-4</v>
       </c>
       <c r="K44">
         <v>42.66</v>
       </c>
     </row>
-    <row r="45" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I45" s="2">
-        <f t="shared" ref="I45:J45" si="16">(I31-$I$24)/I31</f>
+        <f t="shared" ref="I45:J45" si="17">(I31-$I$24)/I31</f>
         <v>-4.8291852704685376E-2</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.2827789150410168E-2</v>
       </c>
       <c r="K45">
         <v>42.66</v>
       </c>
     </row>
-    <row r="46" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I46" s="2">
-        <f t="shared" ref="I46:J46" si="17">(I32-$I$24)/I32</f>
+        <f t="shared" ref="I46:J46" si="18">(I32-$I$24)/I32</f>
         <v>-5.1207928352953493E-2</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.1472742054428385E-2</v>
       </c>
       <c r="K46">
         <v>42.66</v>
       </c>
     </row>
-    <row r="47" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I47" s="2">
-        <f t="shared" ref="I47:J47" si="18">(I33-$I$24)/I33</f>
+        <f t="shared" ref="I47:J47" si="19">(I33-$I$24)/I33</f>
         <v>-5.6479275137367883E-2</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.3425471391326538E-2</v>
       </c>
       <c r="K47">
         <v>42.66</v>
       </c>
     </row>
-    <row r="48" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I48" s="2">
-        <f t="shared" ref="I48:J48" si="19">(I34-$I$24)/I34</f>
+        <f t="shared" ref="I48:J48" si="20">(I34-$I$24)/I34</f>
         <v>-5.481212878369477E-2</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.8935249796863771E-2</v>
       </c>
       <c r="K48">
@@ -3800,11 +6522,11 @@
     </row>
     <row r="49" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I49" s="2">
-        <f t="shared" ref="I49:J49" si="20">(I35-$I$24)/I35</f>
+        <f t="shared" ref="I49:J49" si="21">(I35-$I$24)/I35</f>
         <v>-5.4800344288177365E-2</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.8954840503487495E-2</v>
       </c>
       <c r="K49">

</xml_diff>

<commit_message>
Plots of neural SDE model fits for the write up
</commit_message>
<xml_diff>
--- a/nsde_2021_calibrations/Dynamic_calibration_hedging/Model_market_hedges_comparison.xlsx
+++ b/nsde_2021_calibrations/Dynamic_calibration_hedging/Model_market_hedges_comparison.xlsx
@@ -339,37 +339,37 @@
                   <c:v>42.660000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.930146215100137</c:v>
+                  <c:v>42.376980379853308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.778807317580799</c:v>
+                  <c:v>39.226334476617126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.141504807200363</c:v>
+                  <c:v>39.599655885138532</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.521841879716817</c:v>
+                  <c:v>40.022513627630588</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.458505700660226</c:v>
+                  <c:v>38.959692582411662</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37.08967537676358</c:v>
+                  <c:v>37.320588659628129</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40.694773969609173</c:v>
+                  <c:v>41.458637237722201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.581885704420301</c:v>
+                  <c:v>41.232249675281878</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40.379400717021326</c:v>
+                  <c:v>41.031129673699752</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40.443220964088937</c:v>
+                  <c:v>41.076903995560428</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40.443672805955259</c:v>
+                  <c:v>41.077442649267425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -886,37 +886,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.7406421173819492E-2</c:v>
+                  <c:v>-6.6786169663293933E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.10008540620225891</c:v>
+                  <c:v>-8.7534702622537694E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.98916689619043E-2</c:v>
+                  <c:v>-7.728208860547188E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-7.9403134343638354E-2</c:v>
+                  <c:v>-6.5900068069401782E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.1092474661403095</c:v>
+                  <c:v>-9.4977839205508605E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.15018531617362693</c:v>
+                  <c:v>-0.14306878675115406</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.8291852704685376E-2</c:v>
+                  <c:v>-2.8977381851439936E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.1207928352953493E-2</c:v>
+                  <c:v>-3.4627029472370528E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.6479275137367883E-2</c:v>
+                  <c:v>-3.9698403121090027E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-5.481212878369477E-2</c:v>
+                  <c:v>-3.853980827305474E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-5.4800344288177365E-2</c:v>
+                  <c:v>-3.8526189769041083E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1340,37 +1340,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>765.91399999999999</c:v>
+                  <c:v>765.91400000000021</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>794.91873750320758</c:v>
+                  <c:v>792.1844671348972</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>808.65314100216551</c:v>
+                  <c:v>805.09208778123832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>814.4475161071648</c:v>
+                  <c:v>811.31275089257815</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>818.81323529489202</c:v>
+                  <c:v>815.36367791136172</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>817.46882326592822</c:v>
+                  <c:v>814.90050213931954</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>807.53284111736627</c:v>
+                  <c:v>805.90410832896328</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>814.09505046920879</c:v>
+                  <c:v>811.62770989391208</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>824.73203170593808</c:v>
+                  <c:v>822.27620816035972</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>823.51450529447641</c:v>
+                  <c:v>821.86227580269542</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>828.99464416532646</c:v>
+                  <c:v>826.75741152370892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1430,34 +1430,34 @@
                   <c:v>765.91399999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>797.70053832619624</c:v>
+                  <c:v>799.32967999208347</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>793.50074183852053</c:v>
+                  <c:v>794.81921893078982</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>802.27554623764877</c:v>
+                  <c:v>803.47689822971302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>809.01727175426083</c:v>
+                  <c:v>810.16290145698849</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>803.23220219984466</c:v>
+                  <c:v>804.18199439448665</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>793.09950096392436</c:v>
+                  <c:v>793.67274036510173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>816.44170166468575</c:v>
+                  <c:v>817.77084583938426</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>822.00028586877863</c:v>
+                  <c:v>823.10021378966644</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>817.70392992489099</c:v>
+                  <c:v>818.78749689795268</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>826.97577151279256</c:v>
+                  <c:v>828.02690399556059</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1963,34 +1963,34 @@
                   <c:v>765.91399999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>798.48900892166535</c:v>
+                  <c:v>799.32967999208347</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>794.14201556790408</c:v>
+                  <c:v>794.81921893078982</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>802.871423191654</c:v>
+                  <c:v>803.47689822971302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>809.53766639175933</c:v>
+                  <c:v>810.16290145698849</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>803.76205780797898</c:v>
+                  <c:v>804.18199439448665</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>793.67913754414053</c:v>
+                  <c:v>793.67274036510173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>816.90017361205537</c:v>
+                  <c:v>817.77084583938426</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>822.43004088602652</c:v>
+                  <c:v>823.10021378966644</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>818.12566607762085</c:v>
+                  <c:v>818.78749689795268</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>827.39322096408887</c:v>
+                  <c:v>828.02690399556059</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4461,16 +4461,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1052512</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>414337</xdr:colOff>
+      <xdr:colOff>976312</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4845,10 +4845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Z49"/>
+  <dimension ref="A4:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4859,8 +4859,8 @@
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.140625" customWidth="1"/>
     <col min="13" max="13" width="41.7109375" customWidth="1"/>
@@ -4874,13 +4874,10 @@
     <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="25.28515625" customWidth="1"/>
     <col min="23" max="23" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="L2">
-        <v>-6.4100000000000004E-2</v>
-      </c>
-    </row>
     <row r="4" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
@@ -4960,36 +4957,37 @@
         <v>29.27</v>
       </c>
       <c r="L5">
-        <v>-7.6410000000000006E-2</v>
+        <v>-5.0900000000000001E-2</v>
       </c>
       <c r="M5">
         <v>0.10569248108238501</v>
       </c>
       <c r="O5">
-        <v>0.30840000000000001</v>
+        <f>0.3409</f>
+        <v>0.34089999999999998</v>
       </c>
       <c r="P5">
         <f>-L5*H5</f>
-        <v>58.523488740000005</v>
+        <v>38.985022600000001</v>
       </c>
       <c r="Q5">
         <f>-O5*H5</f>
-        <v>-236.20787759999999</v>
+        <v>-261.10008260000001</v>
       </c>
       <c r="R5">
-        <f>I5+P5+L5*H5</f>
-        <v>42.66</v>
+        <f t="shared" ref="R5:R16" si="0">I5+P5+L5*H5</f>
+        <v>42.660000000000004</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S16" si="0">J5+Q5+O5*H5</f>
+        <f t="shared" ref="S5:S16" si="1">J5+Q5+O5*H5</f>
         <v>29.27000000000001</v>
       </c>
       <c r="T5" s="2">
-        <f t="shared" ref="T5:T16" si="1">(R5-$R$5)/$R$5</f>
+        <f t="shared" ref="T5:T16" si="2">(R5-$R$5)/$R$5</f>
         <v>0</v>
       </c>
       <c r="U5" s="2">
-        <f t="shared" ref="U5:U16" si="2">(S5-$S$5)/$S$5</f>
+        <f t="shared" ref="U5:U16" si="3">(S5-$S$5)/$S$5</f>
         <v>0</v>
       </c>
     </row>
@@ -5018,45 +5016,45 @@
         <v>20.54</v>
       </c>
       <c r="K6">
-        <f>L6-L5</f>
-        <v>-0.45208999999999999</v>
+        <f t="shared" ref="K6:K16" si="4">L6-L5</f>
+        <v>-0.47290000000000004</v>
       </c>
       <c r="L6">
-        <v>-0.52849999999999997</v>
+        <v>-0.52380000000000004</v>
       </c>
       <c r="M6">
         <v>-0.34618849999817403</v>
       </c>
       <c r="N6">
         <f>O6-O5</f>
-        <v>3.6899999999999988E-2</v>
+        <v>2.47E-2</v>
       </c>
       <c r="O6">
-        <v>0.3453</v>
+        <v>0.36559999999999998</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6:P16" si="3">P5*E6-K6*H6</f>
-        <v>420.14473450539469</v>
+        <f t="shared" ref="P6:P16" si="5">P5*E6-K6*H6</f>
+        <v>417.24888637985333</v>
       </c>
       <c r="Q6">
-        <f t="shared" ref="Q6:Q16" si="4">Q5*E6-N6*H6</f>
-        <v>-265.75544005985762</v>
+        <f t="shared" ref="Q6:Q16" si="6">Q5*E6-N6*H6</f>
+        <v>-280.89264118451837</v>
       </c>
       <c r="R6">
-        <f>I6+P6+L6*H6</f>
-        <v>41.513439505394729</v>
+        <f t="shared" si="0"/>
+        <v>42.376980379853308</v>
       </c>
       <c r="S6">
-        <f t="shared" si="0"/>
-        <v>30.97967094014237</v>
+        <f t="shared" si="1"/>
+        <v>32.079830815481614</v>
       </c>
       <c r="T6" s="2">
-        <f t="shared" si="1"/>
-        <v>-2.6876711078416972E-2</v>
+        <f t="shared" si="2"/>
+        <v>-6.6343089579628716E-3</v>
       </c>
       <c r="U6" s="2">
-        <f t="shared" si="2"/>
-        <v>5.8410349851122617E-2</v>
+        <f t="shared" si="3"/>
+        <v>9.5996953040027436E-2</v>
       </c>
     </row>
     <row r="7" spans="4:21" x14ac:dyDescent="0.25">
@@ -5064,14 +5062,14 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E16" si="5">EXP(0.05*(F7-F6)/365)</f>
+        <f t="shared" ref="E7:E16" si="7">EXP(0.05*(F7-F6)/365)</f>
         <v>1.0001369956844217</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G16" si="6">H7-H6</f>
+        <f t="shared" ref="G7:G16" si="8">H7-H6</f>
         <v>0.24400000000002819</v>
       </c>
       <c r="H7">
@@ -5084,45 +5082,46 @@
         <v>16.190000000000001</v>
       </c>
       <c r="K7">
-        <f>L7-L6</f>
-        <v>-0.12140000000000006</v>
+        <f t="shared" si="4"/>
+        <v>-0.12469999999999992</v>
       </c>
       <c r="L7">
-        <v>-0.64990000000000003</v>
+        <f>-0.6485</f>
+        <v>-0.64849999999999997</v>
       </c>
       <c r="M7">
         <v>-0.72825836118487397</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N15" si="7">O7-O6</f>
-        <v>-4.1700000000000015E-2</v>
+        <f t="shared" ref="N7:N15" si="9">O7-O6</f>
+        <v>-6.6399999999999959E-2</v>
       </c>
       <c r="O7">
-        <v>0.30359999999999998</v>
+        <v>0.29920000000000002</v>
       </c>
       <c r="P7">
+        <f t="shared" si="5"/>
+        <v>517.08026347661712</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="6"/>
+        <v>-227.80355266414648</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>39.226334476617126</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="1"/>
+        <v>27.780556135853544</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" si="2"/>
+        <v>-8.0489112128056206E-2</v>
+      </c>
+      <c r="U7" s="2">
         <f t="shared" si="3"/>
-        <v>517.33613212085447</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="4"/>
-        <v>-232.42709360825739</v>
-      </c>
-      <c r="R7">
-        <f>I7+P7+L7*H7</f>
-        <v>38.3620435208544</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="0"/>
-        <v>26.67751679174259</v>
-      </c>
-      <c r="T7" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.10074909702638531</v>
-      </c>
-      <c r="U7" s="2">
-        <f t="shared" si="2"/>
-        <v>-8.8571342953789503E-2</v>
+        <v>-5.0886363653791102E-2</v>
       </c>
     </row>
     <row r="8" spans="4:21" x14ac:dyDescent="0.25">
@@ -5130,14 +5129,14 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0004110433592888</v>
       </c>
       <c r="F8">
         <v>5</v>
       </c>
       <c r="G8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.7859999999999445</v>
       </c>
       <c r="H8">
@@ -5150,45 +5149,46 @@
         <v>14.29</v>
       </c>
       <c r="K8">
-        <f>L8-L7</f>
-        <v>-4.9799999999999955E-2</v>
+        <f t="shared" si="4"/>
+        <v>-4.3399999999999994E-2</v>
       </c>
       <c r="L8">
-        <v>-0.69969999999999999</v>
+        <f>-0.6919</f>
+        <v>-0.69189999999999996</v>
       </c>
       <c r="M8">
         <v>-0.78327956506084595</v>
       </c>
       <c r="N8">
-        <f t="shared" si="7"/>
-        <v>3.6100000000000021E-2</v>
+        <f t="shared" si="9"/>
+        <v>3.8800000000000001E-2</v>
       </c>
       <c r="O8">
-        <v>0.3397</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="P8">
+        <f t="shared" si="5"/>
+        <v>552.35566588513848</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="6"/>
+        <v>-259.24370980169147</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>39.599655885138532</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="1"/>
+        <v>28.116490198308526</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="2"/>
+        <v>-7.1738024258356112E-2</v>
+      </c>
+      <c r="U8" s="2">
         <f t="shared" si="3"/>
-        <v>557.78219970248279</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="4"/>
-        <v>-261.68782122160388</v>
-      </c>
-      <c r="R8">
-        <f>I8+P8+L8*H8</f>
-        <v>38.724569702482881</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="0"/>
-        <v>27.045808778396093</v>
-      </c>
-      <c r="T8" s="2">
-        <f t="shared" si="1"/>
-        <v>-9.2251061826467778E-2</v>
-      </c>
-      <c r="U8" s="2">
-        <f t="shared" si="2"/>
-        <v>-7.5988767393369183E-2</v>
+        <v>-3.9409286016108096E-2</v>
       </c>
     </row>
     <row r="9" spans="4:21" x14ac:dyDescent="0.25">
@@ -5196,14 +5196,14 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F9">
         <v>6</v>
       </c>
       <c r="G9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.5539999999999736</v>
       </c>
       <c r="H9">
@@ -5216,45 +5216,46 @@
         <v>12.95</v>
       </c>
       <c r="K9">
-        <f>L9-L8</f>
-        <v>-0.10160000000000002</v>
+        <f t="shared" si="4"/>
+        <v>-0.10950000000000004</v>
       </c>
       <c r="L9">
-        <v>-0.80130000000000001</v>
+        <f>-0.8014</f>
+        <v>-0.8014</v>
       </c>
       <c r="M9">
         <v>-0.85392030114671702</v>
       </c>
       <c r="N9">
-        <f t="shared" si="7"/>
-        <v>-2.0000000000000018E-2</v>
+        <f t="shared" si="9"/>
+        <v>3.2999999999999696E-3</v>
       </c>
       <c r="O9">
-        <v>0.31969999999999998</v>
+        <v>0.34129999999999999</v>
       </c>
       <c r="P9">
+        <f t="shared" si="5"/>
+        <v>641.5045492276306</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="6"/>
+        <v>-261.96362327114775</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>40.022513627630588</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>28.618226928852209</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="2"/>
+        <v>-6.1825747125396527E-2</v>
+      </c>
+      <c r="U9" s="2">
         <f t="shared" si="3"/>
-        <v>640.50553985668921</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="4"/>
-        <v>-245.45459132377695</v>
-      </c>
-      <c r="R9">
-        <f>I9+P9+L9*H9</f>
-        <v>39.104849656689225</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="0"/>
-        <v>27.556652476223036</v>
-      </c>
-      <c r="T9" s="2">
-        <f t="shared" si="1"/>
-        <v>-8.3336857555339233E-2</v>
-      </c>
-      <c r="U9" s="2">
-        <f t="shared" si="2"/>
-        <v>-5.8535959131430608E-2</v>
+        <v>-2.2267614320047854E-2</v>
       </c>
     </row>
     <row r="10" spans="4:21" x14ac:dyDescent="0.25">
@@ -5262,14 +5263,14 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F10">
         <v>7</v>
       </c>
       <c r="G10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-4.3539999999999281</v>
       </c>
       <c r="H10">
@@ -5282,45 +5283,46 @@
         <v>12.8</v>
       </c>
       <c r="K10">
-        <f>L10-L9</f>
-        <v>1.419999999999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.9000000000000044E-2</v>
       </c>
       <c r="L10">
-        <v>-0.78710000000000002</v>
+        <f>-0.7524</f>
+        <v>-0.75239999999999996</v>
       </c>
       <c r="M10">
         <v>-0.86229317908810799</v>
       </c>
       <c r="N10">
-        <f t="shared" si="7"/>
-        <v>7.3300000000000032E-2</v>
+        <f t="shared" si="9"/>
+        <v>5.9300000000000019E-2</v>
       </c>
       <c r="O10">
-        <v>0.39300000000000002</v>
+        <v>0.40060000000000001</v>
       </c>
       <c r="P10">
+        <f t="shared" si="5"/>
+        <v>601.94653258241169</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="6"/>
+        <v>-309.97914115701144</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>38.959692582411662</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="1"/>
+        <v>26.946318842988603</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="2"/>
+        <v>-8.6739508147874844E-2</v>
+      </c>
+      <c r="U10" s="2">
         <f t="shared" si="3"/>
-        <v>629.10406635149775</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="4"/>
-        <v>-304.79524754350984</v>
-      </c>
-      <c r="R10">
-        <f>I10+P10+L10*H10</f>
-        <v>38.041456351497686</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="0"/>
-        <v>25.981052456490204</v>
-      </c>
-      <c r="T10" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.1082640330169318</v>
-      </c>
-      <c r="U10" s="2">
-        <f t="shared" si="2"/>
-        <v>-0.11236581973043407</v>
+        <v>-7.9387808575722793E-2</v>
       </c>
     </row>
     <row r="11" spans="4:21" x14ac:dyDescent="0.25">
@@ -5328,14 +5330,14 @@
         <v>6</v>
       </c>
       <c r="E11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F11">
         <v>8</v>
       </c>
       <c r="G11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-7.6800000000000637</v>
       </c>
       <c r="H11">
@@ -5348,45 +5350,46 @@
         <v>15.62</v>
       </c>
       <c r="K11">
-        <f>L11-L10</f>
-        <v>6.7500000000000004E-2</v>
+        <f t="shared" si="4"/>
+        <v>6.3199999999999923E-2</v>
       </c>
       <c r="L11">
-        <v>-0.71960000000000002</v>
+        <f>-0.6892</f>
+        <v>-0.68920000000000003</v>
       </c>
       <c r="M11">
         <v>-0.86779167973132199</v>
       </c>
       <c r="N11">
-        <f t="shared" si="7"/>
-        <v>0.18430000000000002</v>
+        <f t="shared" si="9"/>
+        <v>0.18429999999999996</v>
       </c>
       <c r="O11">
-        <v>0.57730000000000004</v>
+        <v>0.58489999999999998</v>
       </c>
       <c r="P11">
+        <f t="shared" si="5"/>
+        <v>551.37925265962815</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="6"/>
+        <v>-457.72331296161065</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>37.320588659628129</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>26.647245038389315</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.1251620098540055</v>
+      </c>
+      <c r="U11" s="2">
         <f t="shared" si="3"/>
-        <v>575.09440089364</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="4"/>
-        <v>-452.53870917705558</v>
-      </c>
-      <c r="R11">
-        <f>I11+P11+L11*H11</f>
-        <v>36.672568893640005</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="0"/>
-        <v>25.741056822944415</v>
-      </c>
-      <c r="T11" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.14035234660947005</v>
-      </c>
-      <c r="U11" s="2">
-        <f t="shared" si="2"/>
-        <v>-0.1205651922465184</v>
+        <v>-8.9605567530259472E-2</v>
       </c>
     </row>
     <row r="12" spans="4:21" x14ac:dyDescent="0.25">
@@ -5394,14 +5397,14 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F12">
         <v>9</v>
       </c>
       <c r="G12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17.639999999999986</v>
       </c>
       <c r="H12">
@@ -5414,46 +5417,47 @@
         <v>10.85</v>
       </c>
       <c r="K12">
-        <f>L12-L11</f>
-        <v>-0.19030000000000002</v>
+        <f t="shared" si="4"/>
+        <v>-0.24269999999999992</v>
       </c>
       <c r="L12">
-        <v>-0.90990000000000004</v>
+        <f>-0.9319</f>
+        <v>-0.93189999999999995</v>
       </c>
       <c r="M12" s="3">
         <f>-0.9</f>
         <v>-0.9</v>
       </c>
       <c r="N12">
-        <f t="shared" si="7"/>
-        <v>-0.21020000000000005</v>
+        <f t="shared" si="9"/>
+        <v>-0.19979999999999998</v>
       </c>
       <c r="O12">
-        <v>0.36709999999999998</v>
+        <v>0.3851</v>
       </c>
       <c r="P12">
+        <f t="shared" si="5"/>
+        <v>750.24065123772209</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="6"/>
+        <v>-294.13783108014559</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>41.458637237722201</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="1"/>
+        <v>32.132174919854435</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.8161339950253234E-2</v>
+      </c>
+      <c r="U12" s="2">
         <f t="shared" si="3"/>
-        <v>731.04030434469757</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="4"/>
-        <v>-280.43429302724655</v>
-      </c>
-      <c r="R12">
-        <f>I12+P12+L12*H12</f>
-        <v>40.277610344697564</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="0"/>
-        <v>31.092632972753449</v>
-      </c>
-      <c r="T12" s="2">
-        <f t="shared" si="1"/>
-        <v>-5.5845983481069686E-2</v>
-      </c>
-      <c r="U12" s="2">
-        <f t="shared" si="2"/>
-        <v>6.2269660838860215E-2</v>
+        <v>9.7785272287476049E-2</v>
       </c>
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">
@@ -5461,14 +5465,14 @@
         <v>8</v>
       </c>
       <c r="E13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0004110433592888</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.5100000000001046</v>
       </c>
       <c r="H13">
@@ -5481,45 +5485,46 @@
         <v>7.05</v>
       </c>
       <c r="K13">
-        <f>L13-L12</f>
-        <v>-6.1199999999999921E-2</v>
+        <f t="shared" si="4"/>
+        <v>-3.9500000000000091E-2</v>
       </c>
       <c r="L13">
-        <v>-0.97109999999999996</v>
+        <f>-0.9714</f>
+        <v>-0.97140000000000004</v>
       </c>
       <c r="M13" s="3">
         <v>-0.93500000000000005</v>
       </c>
       <c r="N13">
-        <f t="shared" si="7"/>
-        <v>6.4400000000000013E-2</v>
+        <f t="shared" si="9"/>
+        <v>7.8400000000000025E-2</v>
       </c>
       <c r="O13">
-        <v>0.43149999999999999</v>
+        <v>0.46350000000000002</v>
       </c>
       <c r="P13">
+        <f t="shared" si="5"/>
+        <v>783.11954767528198</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="6"/>
+        <v>-358.90502248232673</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>41.232249675281878</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="1"/>
+        <v>30.333172517673347</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.3468127630523342E-2</v>
+      </c>
+      <c r="U13" s="2">
         <f t="shared" si="3"/>
-        <v>781.80447760717084</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="4"/>
-        <v>-333.65187168111225</v>
-      </c>
-      <c r="R13">
-        <f>I13+P13+L13*H13</f>
-        <v>40.164550607170895</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="0"/>
-        <v>29.200083318887778</v>
-      </c>
-      <c r="T13" s="2">
-        <f t="shared" si="1"/>
-        <v>-5.8496235181179128E-2</v>
-      </c>
-      <c r="U13" s="2">
-        <f t="shared" si="2"/>
-        <v>-2.3886805982997082E-3</v>
+        <v>3.6322942182211701E-2</v>
       </c>
     </row>
     <row r="14" spans="4:21" x14ac:dyDescent="0.25">
@@ -5527,14 +5532,14 @@
         <v>9</v>
       </c>
       <c r="E14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
       <c r="G14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-4.1400000000001</v>
       </c>
       <c r="H14">
@@ -5547,45 +5552,46 @@
         <v>7.06</v>
       </c>
       <c r="K14">
-        <f>L14-L13</f>
-        <v>-1.8600000000000061E-2</v>
+        <f t="shared" si="4"/>
+        <v>-2.0299999999999985E-2</v>
       </c>
       <c r="L14">
-        <v>-0.98970000000000002</v>
+        <f>-0.9917</f>
+        <v>-0.99170000000000003</v>
       </c>
       <c r="M14" s="3">
         <v>-0.97</v>
       </c>
       <c r="N14">
-        <f t="shared" si="7"/>
-        <v>0.18189999999999995</v>
+        <f t="shared" si="9"/>
+        <v>0.1613</v>
       </c>
       <c r="O14">
-        <v>0.61339999999999995</v>
+        <v>0.62480000000000002</v>
       </c>
       <c r="P14">
+        <f t="shared" si="5"/>
+        <v>799.88156067369971</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="6"/>
+        <v>-491.28954992152404</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>41.031129673699752</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="1"/>
+        <v>28.375114078475917</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.8182614306147486E-2</v>
+      </c>
+      <c r="U14" s="2">
         <f t="shared" si="3"/>
-        <v>797.17157944666462</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="4"/>
-        <v>-482.93379754763174</v>
-      </c>
-      <c r="R14">
-        <f>I14+P14+L14*H14</f>
-        <v>39.96200844666464</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="0"/>
-        <v>27.37796445236819</v>
-      </c>
-      <c r="T14" s="2">
-        <f t="shared" si="1"/>
-        <v>-6.3244058915502971E-2</v>
-      </c>
-      <c r="U14" s="2">
-        <f t="shared" si="2"/>
-        <v>-6.4640777165419203E-2</v>
+        <v>-3.0573485532083795E-2</v>
       </c>
     </row>
     <row r="15" spans="4:21" x14ac:dyDescent="0.25">
@@ -5593,14 +5599,14 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F15">
         <v>14</v>
       </c>
       <c r="G15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.1800000000000637</v>
       </c>
       <c r="H15">
@@ -5614,7 +5620,7 @@
       </c>
       <c r="K15">
         <f>L15-L14</f>
-        <v>-1.0299999999999976E-2</v>
+        <v>-8.2999999999999741E-3</v>
       </c>
       <c r="L15">
         <v>-1</v>
@@ -5623,35 +5629,35 @@
         <v>-1</v>
       </c>
       <c r="N15">
-        <f t="shared" si="7"/>
-        <v>-0.12129999999999996</v>
+        <f t="shared" si="9"/>
+        <v>-0.13280000000000003</v>
       </c>
       <c r="O15">
-        <v>0.49209999999999998</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="P15">
+        <f t="shared" si="5"/>
+        <v>806.8769039955605</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="6"/>
+        <v>-381.18464646966476</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>41.076903995560428</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>30.673473530335229</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.7109610980768287E-2</v>
+      </c>
+      <c r="U15" s="2">
         <f t="shared" si="3"/>
-        <v>805.82577151279247</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="4"/>
-        <v>-382.36826439375716</v>
-      </c>
-      <c r="R15">
-        <f>I15+P15+L15*H15</f>
-        <v>40.025771512792403</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="0"/>
-        <v>29.572816606242839</v>
-      </c>
-      <c r="T15" s="2">
-        <f t="shared" si="1"/>
-        <v>-6.1749378509320059E-2</v>
-      </c>
-      <c r="U15" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0345630551514461E-2</v>
+        <v>4.7949215248897122E-2</v>
       </c>
     </row>
     <row r="16" spans="4:21" x14ac:dyDescent="0.25">
@@ -5659,14 +5665,14 @@
         <v>11</v>
       </c>
       <c r="E16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0001369956844217</v>
       </c>
       <c r="F16">
         <v>15</v>
       </c>
       <c r="G16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>16.110000000000014</v>
       </c>
       <c r="H16">
@@ -5679,7 +5685,7 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <f>L16-L15</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L16">
@@ -5690,34 +5696,34 @@
       </c>
       <c r="N16">
         <f>O16-O15</f>
-        <v>-0.49209999999999998</v>
+        <v>-0.49199999999999999</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" s="4">
+        <f t="shared" si="5"/>
+        <v>-38.732557350732577</v>
+      </c>
+      <c r="Q16" s="3">
+        <f t="shared" si="6"/>
+        <v>34.857372878801073</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>41.077442649267425</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="1"/>
+        <v>34.857372878801073</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.7096984311593494E-2</v>
+      </c>
+      <c r="U16" s="2">
         <f t="shared" si="3"/>
-        <v>-39.783833834114489</v>
-      </c>
-      <c r="Q16" s="3">
-        <f t="shared" si="4"/>
-        <v>33.758164804161083</v>
-      </c>
-      <c r="R16">
-        <f>I16+P16+L16*H16</f>
-        <v>40.026166165885513</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="0"/>
-        <v>33.758164804161083</v>
-      </c>
-      <c r="T16" s="2">
-        <f t="shared" si="1"/>
-        <v>-6.1740127381961642E-2</v>
-      </c>
-      <c r="U16" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1533366861688101</v>
+        <v>0.19089077139737137</v>
       </c>
     </row>
     <row r="17" spans="8:26" x14ac:dyDescent="0.25">
@@ -5786,10 +5792,10 @@
       </c>
       <c r="S22">
         <f>(Q22-Q5-J5)/O5</f>
-        <v>765.91399999999999</v>
+        <v>765.91400000000021</v>
       </c>
       <c r="T22">
-        <f>(R22-P5-I5)/L5</f>
+        <f t="shared" ref="T22:T33" si="10">(R22-P5-I5)/L5</f>
         <v>765.91399999999987</v>
       </c>
       <c r="U22">
@@ -5835,28 +5841,28 @@
       </c>
       <c r="S23">
         <f>(Q23-Q6-J6)/O6</f>
-        <v>794.91873750320758</v>
+        <v>792.1844671348972</v>
       </c>
       <c r="T23">
-        <f>(R23-P6-I6)/L6</f>
-        <v>797.70053832619624</v>
+        <f t="shared" si="10"/>
+        <v>799.32967999208347</v>
       </c>
       <c r="U23">
         <v>799.87</v>
       </c>
       <c r="V23">
-        <f t="shared" ref="V23:V32" si="8">(S23+T23)/2</f>
-        <v>796.30963791470185</v>
+        <f t="shared" ref="V23:V32" si="11">(S23+T23)/2</f>
+        <v>795.75707356349039</v>
       </c>
       <c r="W23" s="2">
-        <f t="shared" ref="W23:W32" si="9">(V23-U23)/V23</f>
-        <v>-4.4710774751159383E-3</v>
+        <f t="shared" ref="W23:W32" si="12">(V23-U23)/V23</f>
+        <v>-5.1685703754934401E-3</v>
       </c>
       <c r="X23">
         <v>814.36442688573084</v>
       </c>
       <c r="Y23">
-        <v>798.48900892166535</v>
+        <v>799.32967999208347</v>
       </c>
       <c r="Z23">
         <v>799.87</v>
@@ -5883,29 +5889,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S24">
-        <f t="shared" ref="S24:S33" si="10">(Q24-Q7-J7)/O7</f>
-        <v>808.65314100216551</v>
+        <f t="shared" ref="S24:S33" si="13">(Q24-Q7-J7)/O7</f>
+        <v>805.09208778123832</v>
       </c>
       <c r="T24">
-        <f>(R24-P7-I7)/L7</f>
-        <v>793.50074183852053</v>
+        <f t="shared" si="10"/>
+        <v>794.81921893078982</v>
       </c>
       <c r="U24">
         <v>800.11400000000003</v>
       </c>
       <c r="V24">
-        <f t="shared" si="8"/>
-        <v>801.07694142034302</v>
+        <f t="shared" si="11"/>
+        <v>799.95565335601407</v>
       </c>
       <c r="W24" s="2">
-        <f t="shared" si="9"/>
-        <v>1.2020585920693842E-3</v>
+        <f t="shared" si="12"/>
+        <v>-1.9794427768797068E-4</v>
       </c>
       <c r="X24">
         <v>802.71164810320226</v>
       </c>
       <c r="Y24">
-        <v>794.14201556790408</v>
+        <v>794.81921893078982</v>
       </c>
       <c r="Z24">
         <v>800.11400000000003</v>
@@ -5914,7 +5920,7 @@
     <row r="25" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
       <c r="I25">
-        <v>41.930146215100137</v>
+        <v>42.376980379853308</v>
       </c>
       <c r="J25">
         <v>47.677803901904383</v>
@@ -5932,29 +5938,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S25">
+        <f t="shared" si="13"/>
+        <v>811.31275089257815</v>
+      </c>
+      <c r="T25">
         <f t="shared" si="10"/>
-        <v>814.4475161071648</v>
-      </c>
-      <c r="T25">
-        <f>(R25-P8-I8)/L8</f>
-        <v>802.27554623764877</v>
+        <v>803.47689822971302</v>
       </c>
       <c r="U25">
         <v>807.9</v>
       </c>
       <c r="V25">
-        <f t="shared" si="8"/>
-        <v>808.36153117240679</v>
+        <f t="shared" si="11"/>
+        <v>807.39482456114558</v>
       </c>
       <c r="W25" s="2">
-        <f t="shared" si="9"/>
-        <v>5.7094648199973886E-4</v>
+        <f t="shared" si="12"/>
+        <v>-6.2568575309976632E-4</v>
       </c>
       <c r="X25">
         <v>810.03525523585859</v>
       </c>
       <c r="Y25">
-        <v>802.871423191654</v>
+        <v>803.47689822971302</v>
       </c>
       <c r="Z25">
         <v>807.9</v>
@@ -5963,7 +5969,7 @@
     <row r="26" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H26" s="1"/>
       <c r="I26">
-        <v>38.778807317580799</v>
+        <v>39.226334476617126</v>
       </c>
       <c r="J26">
         <v>44.551758950573003</v>
@@ -5981,29 +5987,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S26">
+        <f t="shared" si="13"/>
+        <v>815.36367791136172</v>
+      </c>
+      <c r="T26">
         <f t="shared" si="10"/>
-        <v>818.81323529489202</v>
-      </c>
-      <c r="T26">
-        <f>(R26-P9-I9)/L9</f>
-        <v>809.01727175426083</v>
+        <v>810.16290145698849</v>
       </c>
       <c r="U26">
         <v>813.45399999999995</v>
       </c>
       <c r="V26">
-        <f t="shared" si="8"/>
-        <v>813.91525352457643</v>
+        <f t="shared" si="11"/>
+        <v>812.76328968417511</v>
       </c>
       <c r="W26" s="2">
-        <f t="shared" si="9"/>
-        <v>5.6670952237234339E-4</v>
+        <f t="shared" si="12"/>
+        <v>-8.4982961778852246E-4</v>
       </c>
       <c r="X26">
         <v>815.32607118712701</v>
       </c>
       <c r="Y26">
-        <v>809.53766639175933</v>
+        <v>810.16290145698849</v>
       </c>
       <c r="Z26">
         <v>813.45399999999995</v>
@@ -6012,7 +6018,7 @@
     <row r="27" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H27" s="1"/>
       <c r="I27">
-        <v>39.141504807200363</v>
+        <v>39.599655885138532</v>
       </c>
       <c r="J27">
         <v>44.332501792437142</v>
@@ -6030,29 +6036,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S27">
+        <f t="shared" si="13"/>
+        <v>814.90050213931954</v>
+      </c>
+      <c r="T27">
         <f t="shared" si="10"/>
-        <v>817.46882326592822</v>
-      </c>
-      <c r="T27">
-        <f>(R27-P10-I10)/L10</f>
-        <v>803.23220219984466</v>
+        <v>804.18199439448665</v>
       </c>
       <c r="U27">
         <v>809.1</v>
       </c>
       <c r="V27">
-        <f t="shared" si="8"/>
-        <v>810.3505127328865</v>
+        <f t="shared" si="11"/>
+        <v>809.54124826690304</v>
       </c>
       <c r="W27" s="2">
-        <f t="shared" si="9"/>
-        <v>1.5431750992162083E-3</v>
+        <f t="shared" si="12"/>
+        <v>5.4505964686500912E-4</v>
       </c>
       <c r="X27">
         <v>809.99399420984696</v>
       </c>
       <c r="Y27">
-        <v>803.76205780797898</v>
+        <v>804.18199439448665</v>
       </c>
       <c r="Z27">
         <v>809.1</v>
@@ -6061,7 +6067,7 @@
     <row r="28" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H28" s="1"/>
       <c r="I28">
-        <v>39.521841879716817</v>
+        <v>40.022513627630588</v>
       </c>
       <c r="J28">
         <v>44.258599591879602</v>
@@ -6079,29 +6085,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S28">
+        <f t="shared" si="13"/>
+        <v>805.90410832896328</v>
+      </c>
+      <c r="T28">
         <f t="shared" si="10"/>
-        <v>807.53284111736627</v>
-      </c>
-      <c r="T28">
-        <f>(R28-P11-I11)/L11</f>
-        <v>793.09950096392436</v>
+        <v>793.67274036510173</v>
       </c>
       <c r="U28">
         <v>801.42</v>
       </c>
       <c r="V28">
-        <f t="shared" si="8"/>
-        <v>800.31617104064526</v>
+        <f t="shared" si="11"/>
+        <v>799.78842434703256</v>
       </c>
       <c r="W28" s="2">
-        <f t="shared" si="9"/>
-        <v>-1.3792411040744058E-3</v>
+        <f t="shared" si="12"/>
+        <v>-2.0400090865274256E-3</v>
       </c>
       <c r="X28">
         <v>801.40681048488716</v>
       </c>
       <c r="Y28">
-        <v>793.67913754414053</v>
+        <v>793.67274036510173</v>
       </c>
       <c r="Z28">
         <v>801.42</v>
@@ -6110,7 +6116,7 @@
     <row r="29" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H29" s="1"/>
       <c r="I29">
-        <v>38.458505700660226</v>
+        <v>38.959692582411662</v>
       </c>
       <c r="J29">
         <v>43.430885109295218</v>
@@ -6128,29 +6134,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S29">
+        <f t="shared" si="13"/>
+        <v>811.62770989391208</v>
+      </c>
+      <c r="T29">
         <f t="shared" si="10"/>
-        <v>814.09505046920879</v>
-      </c>
-      <c r="T29">
-        <f>(R29-P12-I12)/L12</f>
-        <v>816.44170166468575</v>
+        <v>817.77084583938426</v>
       </c>
       <c r="U29">
         <v>819.06</v>
       </c>
       <c r="V29">
-        <f t="shared" si="8"/>
-        <v>815.26837606694721</v>
+        <f t="shared" si="11"/>
+        <v>814.69927786664812</v>
       </c>
       <c r="W29" s="2">
-        <f t="shared" si="9"/>
-        <v>-4.6507678261046362E-3</v>
+        <f t="shared" si="12"/>
+        <v>-5.3525543127652085E-3</v>
       </c>
       <c r="X29">
         <v>820.1673147534442</v>
       </c>
       <c r="Y29">
-        <v>816.90017361205537</v>
+        <v>817.77084583938426</v>
       </c>
       <c r="Z29">
         <v>819.06</v>
@@ -6159,7 +6165,7 @@
     <row r="30" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H30" s="1"/>
       <c r="I30">
-        <v>37.08967537676358</v>
+        <v>37.320588659628129</v>
       </c>
       <c r="J30">
         <v>42.648554248525443</v>
@@ -6177,29 +6183,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S30">
+        <f t="shared" si="13"/>
+        <v>822.27620816035972</v>
+      </c>
+      <c r="T30">
         <f t="shared" si="10"/>
-        <v>824.73203170593808</v>
-      </c>
-      <c r="T30">
-        <f>(R30-P13-I13)/L13</f>
-        <v>822.00028586877863</v>
+        <v>823.10021378966644</v>
       </c>
       <c r="U30">
         <v>824.57</v>
       </c>
       <c r="V30">
-        <f t="shared" si="8"/>
-        <v>823.36615878735836</v>
+        <f t="shared" si="11"/>
+        <v>822.68821097501313</v>
       </c>
       <c r="W30" s="2">
-        <f t="shared" si="9"/>
-        <v>-1.4620970266918563E-3</v>
+        <f t="shared" si="12"/>
+        <v>-2.2873659788520649E-3</v>
       </c>
       <c r="X30">
         <v>825.57120686645715</v>
       </c>
       <c r="Y30">
-        <v>822.43004088602652</v>
+        <v>823.10021378966644</v>
       </c>
       <c r="Z30">
         <v>824.57</v>
@@ -6208,7 +6214,7 @@
     <row r="31" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H31" s="1"/>
       <c r="I31">
-        <v>40.694773969609173</v>
+        <v>41.458637237722201</v>
       </c>
       <c r="J31">
         <v>43.656583278099788</v>
@@ -6226,29 +6232,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S31">
+        <f t="shared" si="13"/>
+        <v>821.86227580269542</v>
+      </c>
+      <c r="T31">
         <f t="shared" si="10"/>
-        <v>823.51450529447641</v>
-      </c>
-      <c r="T31">
-        <f>(R31-P14-I14)/L14</f>
-        <v>817.70392992489099</v>
+        <v>818.78749689795268</v>
       </c>
       <c r="U31">
         <v>820.43</v>
       </c>
       <c r="V31">
-        <f t="shared" si="8"/>
-        <v>820.6092176096837</v>
+        <f t="shared" si="11"/>
+        <v>820.32488635032405</v>
       </c>
       <c r="W31" s="2">
-        <f t="shared" si="9"/>
-        <v>2.1839580379779503E-4</v>
+        <f t="shared" si="12"/>
+        <v>-1.2813660956155685E-4</v>
       </c>
       <c r="X31">
         <v>821.02847878721127</v>
       </c>
       <c r="Y31">
-        <v>818.12566607762085</v>
+        <v>818.78749689795268</v>
       </c>
       <c r="Z31">
         <v>820.43</v>
@@ -6257,7 +6263,7 @@
     <row r="32" spans="8:26" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
       <c r="I32">
-        <v>40.581885704420301</v>
+        <v>41.232249675281878</v>
       </c>
       <c r="J32">
         <v>43.596128420137347</v>
@@ -6275,29 +6281,29 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S32">
+        <f t="shared" si="13"/>
+        <v>826.75741152370892</v>
+      </c>
+      <c r="T32">
         <f t="shared" si="10"/>
-        <v>828.99464416532646</v>
-      </c>
-      <c r="T32">
-        <f>(R32-P15-I15)/L15</f>
-        <v>826.97577151279256</v>
+        <v>828.02690399556059</v>
       </c>
       <c r="U32">
         <v>829.61</v>
       </c>
       <c r="V32">
-        <f t="shared" si="8"/>
-        <v>827.98520783905951</v>
+        <f t="shared" si="11"/>
+        <v>827.39215775963476</v>
       </c>
       <c r="W32" s="2">
-        <f t="shared" si="9"/>
-        <v>-1.9623444302598238E-3</v>
+        <f t="shared" si="12"/>
+        <v>-2.6805212251112026E-3</v>
       </c>
       <c r="X32">
         <v>830.43336844348642</v>
       </c>
       <c r="Y32">
-        <v>827.39322096408887</v>
+        <v>828.02690399556059</v>
       </c>
       <c r="Z32">
         <v>829.61</v>
@@ -6305,7 +6311,7 @@
     </row>
     <row r="33" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I33">
-        <v>40.379400717021326</v>
+        <v>41.031129673699752</v>
       </c>
       <c r="J33">
         <v>43.240524423594934</v>
@@ -6323,11 +6329,11 @@
         <v>42.660000000000004</v>
       </c>
       <c r="S33" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T33" t="e">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T33" t="e">
-        <f>(R33-P16-I16)/L16</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U33">
@@ -6346,7 +6352,7 @@
     </row>
     <row r="34" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I34">
-        <v>40.443220964088937</v>
+        <v>41.076903995560428</v>
       </c>
       <c r="J34">
         <v>43.483368443486484</v>
@@ -6357,7 +6363,7 @@
     </row>
     <row r="35" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I35">
-        <v>40.443672805955259</v>
+        <v>41.077442649267425</v>
       </c>
       <c r="J35">
         <v>43.484236772437441</v>
@@ -6392,11 +6398,11 @@
     </row>
     <row r="39" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I39" s="2">
-        <f t="shared" ref="I39:J39" si="11">(I25-$I$24)/I25</f>
-        <v>-1.7406421173819492E-2</v>
+        <f t="shared" ref="I39:J39" si="14">(I25-$I$24)/I25</f>
+        <v>-6.6786169663293933E-3</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.10524402324042351</v>
       </c>
       <c r="K39">
@@ -6405,11 +6411,11 @@
     </row>
     <row r="40" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I40" s="2">
-        <f t="shared" ref="I40:J40" si="12">(I26-$I$24)/I26</f>
-        <v>-0.10008540620225891</v>
+        <f t="shared" ref="I40:J40" si="15">(I26-$I$24)/I26</f>
+        <v>-8.7534702622537694E-2</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>4.2462048528134899E-2</v>
       </c>
       <c r="K40">
@@ -6418,11 +6424,11 @@
     </row>
     <row r="41" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I41" s="2">
-        <f t="shared" ref="I41:J41" si="13">(I27-$I$24)/I27</f>
-        <v>-8.98916689619043E-2</v>
+        <f t="shared" ref="I41:J41" si="16">(I27-$I$24)/I27</f>
+        <v>-7.728208860547188E-2</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>3.7726311956580293E-2</v>
       </c>
       <c r="K41">
@@ -6431,11 +6437,11 @@
     </row>
     <row r="42" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I42" s="2">
-        <f t="shared" ref="I42:J42" si="14">(I28-$I$24)/I28</f>
-        <v>-7.9403134343638354E-2</v>
+        <f t="shared" ref="I42:J42" si="17">(I28-$I$24)/I28</f>
+        <v>-6.5900068069401782E-2</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.6119524942513158E-2</v>
       </c>
       <c r="K42">
@@ -6444,11 +6450,11 @@
     </row>
     <row r="43" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I43" s="2">
-        <f t="shared" ref="I43:J43" si="15">(I29-$I$24)/I29</f>
-        <v>-0.1092474661403095</v>
+        <f t="shared" ref="I43:J43" si="18">(I29-$I$24)/I29</f>
+        <v>-9.4977839205508605E-2</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1.7749698339217756E-2</v>
       </c>
       <c r="K43">
@@ -6457,11 +6463,11 @@
     </row>
     <row r="44" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I44" s="2">
-        <f t="shared" ref="I44:J44" si="16">(I30-$I$24)/I30</f>
-        <v>-0.15018531617362693</v>
+        <f t="shared" ref="I44:J44" si="19">(I30-$I$24)/I30</f>
+        <v>-0.14306878675115406</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>-2.6837372746244225E-4</v>
       </c>
       <c r="K44">
@@ -6470,11 +6476,11 @@
     </row>
     <row r="45" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I45" s="2">
-        <f t="shared" ref="I45:J45" si="17">(I31-$I$24)/I31</f>
-        <v>-4.8291852704685376E-2</v>
+        <f t="shared" ref="I45:J45" si="20">(I31-$I$24)/I31</f>
+        <v>-2.8977381851439936E-2</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>2.2827789150410168E-2</v>
       </c>
       <c r="K45">
@@ -6483,11 +6489,11 @@
     </row>
     <row r="46" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I46" s="2">
-        <f t="shared" ref="I46:J46" si="18">(I32-$I$24)/I32</f>
-        <v>-5.1207928352953493E-2</v>
+        <f t="shared" ref="I46:J46" si="21">(I32-$I$24)/I32</f>
+        <v>-3.4627029472370528E-2</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>2.1472742054428385E-2</v>
       </c>
       <c r="K46">
@@ -6496,11 +6502,11 @@
     </row>
     <row r="47" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I47" s="2">
-        <f t="shared" ref="I47:J47" si="19">(I33-$I$24)/I33</f>
-        <v>-5.6479275137367883E-2</v>
+        <f t="shared" ref="I47:J47" si="22">(I33-$I$24)/I33</f>
+        <v>-3.9698403121090027E-2</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>1.3425471391326538E-2</v>
       </c>
       <c r="K47">
@@ -6509,11 +6515,11 @@
     </row>
     <row r="48" spans="9:26" x14ac:dyDescent="0.25">
       <c r="I48" s="2">
-        <f t="shared" ref="I48:J48" si="20">(I34-$I$24)/I34</f>
-        <v>-5.481212878369477E-2</v>
+        <f t="shared" ref="I48:J48" si="23">(I34-$I$24)/I34</f>
+        <v>-3.853980827305474E-2</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1.8935249796863771E-2</v>
       </c>
       <c r="K48">
@@ -6522,11 +6528,11 @@
     </row>
     <row r="49" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I49" s="2">
-        <f t="shared" ref="I49:J49" si="21">(I35-$I$24)/I35</f>
-        <v>-5.4800344288177365E-2</v>
+        <f t="shared" ref="I49:J49" si="24">(I35-$I$24)/I35</f>
+        <v>-3.8526189769041083E-2</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>1.8954840503487495E-2</v>
       </c>
       <c r="K49">

</xml_diff>